<commit_message>
Update Mario running and fixed Enemyspawner
</commit_message>
<xml_diff>
--- a/Super_Mario_Bros3-main/Super_Mario_Bros3/Object_type_Enemy_Spawner.xlsx
+++ b/Super_Mario_Bros3-main/Super_Mario_Bros3/Object_type_Enemy_Spawner.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\StudyInUIT\Nhập môn phát triển game\My_Project\Mario_Bors_3\Super_Mario_Bros3-main\Super_Mario_Bros3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{611AC797-C9BC-40D9-8228-B1B71944C05D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04D822D-FF07-4258-99FB-4924A6A9FE5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{820C61C8-622B-4395-993E-4E378A502B8B}"/>
+    <workbookView xWindow="1820" yWindow="1820" windowWidth="14400" windowHeight="7810" xr2:uid="{820C61C8-622B-4395-993E-4E378A502B8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>type</t>
   </si>
@@ -63,7 +63,13 @@
     <t>enemyY</t>
   </si>
   <si>
-    <t>enemyAnimSetId</t>
+    <t>eAniSet</t>
+  </si>
+  <si>
+    <t>minPatX</t>
+  </si>
+  <si>
+    <t>maxPatX</t>
   </si>
 </sst>
 </file>
@@ -415,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C37A1A99-4A68-4593-AD00-0B5E4539E5C0}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="A2" sqref="A2:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -426,7 +432,7 @@
     <col min="10" max="10" width="17.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -457,35 +463,37 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>9</v>
       </c>
       <c r="B2">
-        <f>H2 - 160</f>
-        <v>368</v>
+        <v>40</v>
       </c>
       <c r="C2">
-        <f>I2-100</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <f>H2 + 160</f>
-        <v>688</v>
+        <v>340</v>
       </c>
       <c r="F2">
-        <f xml:space="preserve"> I2 + 16</f>
         <v>150</v>
       </c>
       <c r="G2">
         <v>20</v>
       </c>
       <c r="H2">
-        <v>528</v>
+        <v>200</v>
       </c>
       <c r="I2">
         <v>134</v>
@@ -493,77 +501,125 @@
       <c r="J2">
         <v>88</v>
       </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>330</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>9</v>
       </c>
       <c r="B3">
-        <f>H3 - 160</f>
-        <v>672</v>
+        <v>368</v>
       </c>
       <c r="C3">
-        <f>I3-100</f>
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E4" si="0">H3 + 160</f>
-        <v>992</v>
+        <v>688</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F4" si="1" xml:space="preserve"> I3 + 16</f>
-        <v>131</v>
+        <v>150</v>
       </c>
       <c r="G3">
         <v>20</v>
       </c>
       <c r="H3">
-        <v>832</v>
+        <v>528</v>
       </c>
       <c r="I3">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="J3">
         <v>88</v>
       </c>
+      <c r="K3">
+        <v>390</v>
+      </c>
+      <c r="L3">
+        <v>600</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>9</v>
       </c>
       <c r="B4">
-        <f>H4 - 160</f>
-        <v>720</v>
+        <v>672</v>
       </c>
       <c r="C4">
-        <f>I4-100</f>
         <v>15</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
-        <v>1040</v>
+        <v>992</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
         <v>131</v>
       </c>
       <c r="G4">
         <v>20</v>
       </c>
       <c r="H4">
-        <v>880</v>
+        <v>832</v>
       </c>
       <c r="I4">
         <v>115</v>
       </c>
       <c r="J4">
         <v>88</v>
+      </c>
+      <c r="K4">
+        <v>680</v>
+      </c>
+      <c r="L4">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>720</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1040</v>
+      </c>
+      <c r="F5">
+        <v>131</v>
+      </c>
+      <c r="G5">
+        <v>20</v>
+      </c>
+      <c r="H5">
+        <v>880</v>
+      </c>
+      <c r="I5">
+        <v>115</v>
+      </c>
+      <c r="J5">
+        <v>88</v>
+      </c>
+      <c r="K5">
+        <v>680</v>
+      </c>
+      <c r="L5">
+        <v>1080</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
almost finish para goomba (just change a little bit height and animation)
</commit_message>
<xml_diff>
--- a/Super_Mario_Bros3-main/Super_Mario_Bros3/Object_type_Enemy_Spawner.xlsx
+++ b/Super_Mario_Bros3-main/Super_Mario_Bros3/Object_type_Enemy_Spawner.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\StudyInUIT\Nhập môn phát triển game\My_Project\Mario_Bors_3\Super_Mario_Bros3-main\Super_Mario_Bros3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04D822D-FF07-4258-99FB-4924A6A9FE5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBABFE44-046A-4744-8C0E-8B8B454DB9F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="1820" windowWidth="14400" windowHeight="7810" xr2:uid="{820C61C8-622B-4395-993E-4E378A502B8B}"/>
+    <workbookView minimized="1" xWindow="1820" yWindow="1820" windowWidth="14400" windowHeight="7810" xr2:uid="{820C61C8-622B-4395-993E-4E378A502B8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -421,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C37A1A99-4A68-4593-AD00-0B5E4539E5C0}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -622,6 +622,48 @@
         <v>1080</v>
       </c>
     </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <f>H7 - 160</f>
+        <v>784</v>
+      </c>
+      <c r="C7">
+        <f>I7 - 100</f>
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f xml:space="preserve"> H7 + 160</f>
+        <v>1104</v>
+      </c>
+      <c r="F7">
+        <f>I7 + 16</f>
+        <v>131</v>
+      </c>
+      <c r="G7">
+        <v>21</v>
+      </c>
+      <c r="H7">
+        <v>944</v>
+      </c>
+      <c r="I7">
+        <v>115</v>
+      </c>
+      <c r="J7">
+        <v>88</v>
+      </c>
+      <c r="K7">
+        <v>680</v>
+      </c>
+      <c r="L7">
+        <v>1080</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Koopases have animations but less logic
</commit_message>
<xml_diff>
--- a/Super_Mario_Bros3-main/Super_Mario_Bros3/Object_type_Enemy_Spawner.xlsx
+++ b/Super_Mario_Bros3-main/Super_Mario_Bros3/Object_type_Enemy_Spawner.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\StudyInUIT\Nhập môn phát triển game\My_Project\Mario_Bors_3\Super_Mario_Bros3-main\Super_Mario_Bros3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBABFE44-046A-4744-8C0E-8B8B454DB9F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B3A75D-9EE7-485A-96A3-A797AAF080C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1820" yWindow="1820" windowWidth="14400" windowHeight="7810" xr2:uid="{820C61C8-622B-4395-993E-4E378A502B8B}"/>
+    <workbookView xWindow="1060" yWindow="2710" windowWidth="14400" windowHeight="7810" xr2:uid="{820C61C8-622B-4395-993E-4E378A502B8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -421,15 +421,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C37A1A99-4A68-4593-AD00-0B5E4539E5C0}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:L7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="10" max="10" width="17.81640625" customWidth="1"/>
+    <col min="10" max="10" width="8.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -664,6 +664,258 @@
         <v>1080</v>
       </c>
     </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ref="B8:B11" si="0">H9 - 160</f>
+        <v>1168</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C8:C11" si="1">I9 - 100</f>
+        <v>-73</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ref="E8:E11" si="2" xml:space="preserve"> H9 + 160</f>
+        <v>1488</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F8:F11" si="3">I9 + 16</f>
+        <v>43</v>
+      </c>
+      <c r="G9">
+        <v>301</v>
+      </c>
+      <c r="H9">
+        <v>1328</v>
+      </c>
+      <c r="I9">
+        <v>27</v>
+      </c>
+      <c r="J9">
+        <v>89</v>
+      </c>
+      <c r="K9">
+        <v>1100</v>
+      </c>
+      <c r="L9">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>1216</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>-73</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>1536</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="G10">
+        <v>301</v>
+      </c>
+      <c r="H10">
+        <v>1376</v>
+      </c>
+      <c r="I10">
+        <v>27</v>
+      </c>
+      <c r="J10">
+        <v>89</v>
+      </c>
+      <c r="K10">
+        <v>1100</v>
+      </c>
+      <c r="L10">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>1265</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>-73</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>1585</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="G11">
+        <v>301</v>
+      </c>
+      <c r="H11">
+        <v>1425</v>
+      </c>
+      <c r="I11">
+        <v>27</v>
+      </c>
+      <c r="J11">
+        <v>89</v>
+      </c>
+      <c r="K11">
+        <v>1100</v>
+      </c>
+      <c r="L11">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <f t="shared" ref="B12:B13" si="4">H13 - 160</f>
+        <v>1312</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C12:C13" si="5">I13 - 100</f>
+        <v>23</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ref="E12:E13" si="6" xml:space="preserve"> H13 + 160</f>
+        <v>1632</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ref="F12:F13" si="7">I13 + 16</f>
+        <v>139</v>
+      </c>
+      <c r="G13">
+        <v>30</v>
+      </c>
+      <c r="H13">
+        <v>1472</v>
+      </c>
+      <c r="I13">
+        <v>123</v>
+      </c>
+      <c r="J13">
+        <v>89</v>
+      </c>
+      <c r="K13">
+        <v>1160</v>
+      </c>
+      <c r="L13">
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ref="B14:B16" si="8">H15 - 160</f>
+        <v>416</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C14:C16" si="9">I15 - 100</f>
+        <v>-9</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ref="E14:E16" si="10" xml:space="preserve"> H15 + 160</f>
+        <v>736</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ref="F14:F16" si="11">I15 + 16</f>
+        <v>107</v>
+      </c>
+      <c r="G15">
+        <v>31</v>
+      </c>
+      <c r="H15">
+        <v>576</v>
+      </c>
+      <c r="I15">
+        <v>91</v>
+      </c>
+      <c r="J15">
+        <v>89</v>
+      </c>
+      <c r="K15">
+        <v>515</v>
+      </c>
+      <c r="L15">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="8"/>
+        <v>1936</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="9"/>
+        <v>-9</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="10"/>
+        <v>2256</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="11"/>
+        <v>107</v>
+      </c>
+      <c r="G16">
+        <v>31</v>
+      </c>
+      <c r="H16">
+        <v>2096</v>
+      </c>
+      <c r="I16">
+        <v>91</v>
+      </c>
+      <c r="J16">
+        <v>89</v>
+      </c>
+      <c r="K16">
+        <v>2090</v>
+      </c>
+      <c r="L16">
+        <v>2104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>